<commit_message>
Changed MP LAUNCHPAD to reflect new water use from Jason Smesrud
 - removed (HW) designation for step 0 DCMs (Step 0 water use is now consumptive use)
 - updated all step0 and prescription habitat water use per J. Smesrud's calculations
</commit_message>
<xml_diff>
--- a/MP LAUNCHPAD PROJECT.xlsx
+++ b/MP LAUNCHPAD PROJECT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/code/master_proj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C4551F-EEE6-CB44-B180-21EE3F5AF201}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AF7A5B-4B3C-3E41-8D2E-F4E6B0339095}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3140" yWindow="1040" windowWidth="25420" windowHeight="20220" xr2:uid="{82E405D1-4FF9-4B4B-A5DF-847AC901B550}"/>
+    <workbookView xWindow="3140" yWindow="1040" windowWidth="31280" windowHeight="20220" activeTab="6" xr2:uid="{82E405D1-4FF9-4B4B-A5DF-847AC901B550}"/>
   </bookViews>
   <sheets>
     <sheet name="MP_new" sheetId="1" r:id="rId1"/>
@@ -4711,16 +4711,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="65" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="74" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="74" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="61" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4741,12 +4802,6 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="71" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -4761,82 +4816,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="65" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -4898,6 +4877,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5346,960 +5346,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>w/o GW</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>MP_new!$A$13:$A$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>MP_new!$I$13:$I$18</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4926.6207202706355</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D0D5-C846-912D-CB91A199CB47}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>w/ GW</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>MP_new!$A$13:$A$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>MP_new!$K$13:$K$18</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9926.6207202706355</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D0D5-C846-912D-CB91A199CB47}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="196036608"/>
-        <c:axId val="160822912"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="196036608"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Step</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160822912"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="160822912"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Total</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> </a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Water Savings (a-f/y)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196036608"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:overlay val="1"/>
-      <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.1453912948381452"/>
-          <c:y val="5.1400554097404488E-2"/>
-          <c:w val="0.81701159230096243"/>
-          <c:h val="0.82202719451735196"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>MP_new!$B$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>BWF</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>MP_new!$A$13:$A$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>MP_new!$B$13:$B$18</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>2.1005477801387333</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0785334641965729</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4242-2D4D-90F8-71367A6093A9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>MP_new!$C$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>MWF</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>MP_new!$A$13:$A$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>MP_new!$C$13:$C$18</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.97824344759700355</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.9382694221923642</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-4242-2D4D-90F8-71367A6093A9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>MP_new!$D$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Plover</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>MP_new!$A$13:$A$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>MP_new!$D$13:$D$18</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.99961756413569214</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0176368154509927</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-4242-2D4D-90F8-71367A6093A9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>MP_new!$E$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>MSB</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>MP_new!$A$13:$A$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>MP_new!$E$13:$E$18</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.90639366309330827</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.90000167824924227</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-4242-2D4D-90F8-71367A6093A9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>MP_new!$F$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Meadow</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>MP_new!$A$13:$A$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>MP_new!$F$13:$F$18</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.3860992059091843</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.3400570388796187</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-4242-2D4D-90F8-71367A6093A9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="196038144"/>
-        <c:axId val="160824640"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="196038144"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Step</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160824640"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="160824640"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="0.5"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>%</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> of Base Area</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196038144"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-        <c:majorUnit val="0.1"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>MP_new!$A$3:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Base</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>MP_new!$G$3:$G$9</c:f>
-              <c:numCache>
-                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>73351</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>64619.055153407739</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>59692.434433137103</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-188D-C64B-B0F2-7C3CB2224891}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="196272640"/>
-        <c:axId val="196306624"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="196272640"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Step</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196306624"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="196306624"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Total</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> </a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Water Demand (a-f/y)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196272640"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
@@ -6587,7 +5633,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -7242,119 +6288,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>195262</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>187324</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>530225</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>12699</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>50800</xdr:colOff>
       <xdr:row>20</xdr:row>
@@ -7588,7 +6521,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7629,7 +6562,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8062,8 +6995,8 @@
   </sheetPr>
   <dimension ref="A1:CP191"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:K18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L40" sqref="L22:L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8435,7 +7368,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="121">
-        <f t="shared" ref="B12:G18" si="0">B3/B$3</f>
+        <f t="shared" ref="B12:G14" si="0">B3/B$3</f>
         <v>1</v>
       </c>
       <c r="C12" s="121">
@@ -8510,14 +7443,14 @@
         <v>0.88095670343155152</v>
       </c>
       <c r="H13" s="145">
-        <f t="shared" ref="H13:H18" si="1">$G3-$G4</f>
+        <f t="shared" ref="H13:H14" si="1">$G3-$G4</f>
         <v>8731.9448465922615</v>
       </c>
       <c r="I13" s="145">
         <v>0</v>
       </c>
       <c r="J13" s="145">
-        <f t="shared" ref="J13:J18" si="2">G3-(G4 -J4)</f>
+        <f t="shared" ref="J13:J14" si="2">G3-(G4 -J4)</f>
         <v>8731.9448465922615</v>
       </c>
       <c r="K13" s="145">
@@ -14891,7 +13824,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;P&amp;R&amp;D</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -17380,16 +16312,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="476" t="s">
+      <c r="A1" s="453" t="s">
         <v>171</v>
       </c>
-      <c r="B1" s="477"/>
+      <c r="B1" s="454"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="478" t="s">
+      <c r="A2" s="455" t="s">
         <v>172</v>
       </c>
-      <c r="B2" s="479"/>
+      <c r="B2" s="456"/>
     </row>
     <row r="3" spans="1:40" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="X3" s="239" t="s">
@@ -17397,33 +16329,33 @@
       </c>
     </row>
     <row r="4" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="483" t="s">
+      <c r="A4" s="463" t="s">
         <v>174</v>
       </c>
-      <c r="B4" s="484"/>
+      <c r="B4" s="464"/>
       <c r="C4" s="67"/>
-      <c r="D4" s="487" t="s">
+      <c r="D4" s="467" t="s">
         <v>175</v>
       </c>
-      <c r="E4" s="480" t="s">
+      <c r="E4" s="457" t="s">
         <v>176</v>
       </c>
-      <c r="F4" s="481"/>
-      <c r="G4" s="481"/>
-      <c r="H4" s="481"/>
-      <c r="I4" s="481"/>
-      <c r="J4" s="481"/>
-      <c r="K4" s="481"/>
-      <c r="L4" s="481"/>
-      <c r="M4" s="481"/>
-      <c r="N4" s="481"/>
-      <c r="O4" s="481"/>
-      <c r="P4" s="481"/>
-      <c r="Q4" s="481"/>
-      <c r="R4" s="481"/>
-      <c r="S4" s="481"/>
-      <c r="T4" s="481"/>
-      <c r="U4" s="482"/>
+      <c r="F4" s="458"/>
+      <c r="G4" s="458"/>
+      <c r="H4" s="458"/>
+      <c r="I4" s="458"/>
+      <c r="J4" s="458"/>
+      <c r="K4" s="458"/>
+      <c r="L4" s="458"/>
+      <c r="M4" s="458"/>
+      <c r="N4" s="458"/>
+      <c r="O4" s="458"/>
+      <c r="P4" s="458"/>
+      <c r="Q4" s="458"/>
+      <c r="R4" s="458"/>
+      <c r="S4" s="458"/>
+      <c r="T4" s="458"/>
+      <c r="U4" s="459"/>
       <c r="Y4" s="239">
         <f t="shared" ref="Y4:AN4" si="0">E5</f>
         <v>2020</v>
@@ -17490,12 +16422,12 @@
       </c>
     </row>
     <row r="5" spans="1:40" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="485"/>
-      <c r="B5" s="486"/>
+      <c r="A5" s="465"/>
+      <c r="B5" s="466"/>
       <c r="C5" s="68" t="s">
         <v>177</v>
       </c>
-      <c r="D5" s="488"/>
+      <c r="D5" s="468"/>
       <c r="E5" s="69">
         <f>'Step Cost Analysis'!E5</f>
         <v>2020</v>
@@ -17633,10 +16565,10 @@
       </c>
     </row>
     <row r="6" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="455" t="s">
+      <c r="A6" s="469" t="s">
         <v>179</v>
       </c>
-      <c r="B6" s="456"/>
+      <c r="B6" s="470"/>
       <c r="C6" s="160">
         <v>10</v>
       </c>
@@ -18154,12 +17086,12 @@
       </c>
     </row>
     <row r="12" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="470" t="s">
+      <c r="A12" s="460" t="s">
         <v>190</v>
       </c>
-      <c r="B12" s="471"/>
-      <c r="C12" s="471"/>
-      <c r="D12" s="472"/>
+      <c r="B12" s="461"/>
+      <c r="C12" s="461"/>
+      <c r="D12" s="462"/>
       <c r="E12" s="279">
         <f t="shared" ref="E12:T12" si="8">SUM(E6:E11)</f>
         <v>1500000</v>
@@ -18294,12 +17226,12 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="470" t="s">
+      <c r="A13" s="460" t="s">
         <v>191</v>
       </c>
-      <c r="B13" s="471"/>
-      <c r="C13" s="471"/>
-      <c r="D13" s="472"/>
+      <c r="B13" s="461"/>
+      <c r="C13" s="461"/>
+      <c r="D13" s="462"/>
       <c r="E13" s="279"/>
       <c r="F13" s="279"/>
       <c r="G13" s="279"/>
@@ -18392,10 +17324,10 @@
       </c>
     </row>
     <row r="14" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="455" t="s">
+      <c r="A14" s="469" t="s">
         <v>192</v>
       </c>
-      <c r="B14" s="456"/>
+      <c r="B14" s="470"/>
       <c r="C14" s="162">
         <v>10</v>
       </c>
@@ -18910,12 +17842,12 @@
       </c>
     </row>
     <row r="20" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="470" t="s">
+      <c r="A20" s="460" t="s">
         <v>195</v>
       </c>
-      <c r="B20" s="471"/>
-      <c r="C20" s="471"/>
-      <c r="D20" s="472"/>
+      <c r="B20" s="461"/>
+      <c r="C20" s="461"/>
+      <c r="D20" s="462"/>
       <c r="E20" s="279">
         <f t="shared" ref="E20:T20" si="15">SUM(E14:E19)</f>
         <v>0</v>
@@ -18986,12 +17918,12 @@
       </c>
     </row>
     <row r="21" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="470" t="s">
+      <c r="A21" s="460" t="s">
         <v>196</v>
       </c>
-      <c r="B21" s="471"/>
-      <c r="C21" s="471"/>
-      <c r="D21" s="472"/>
+      <c r="B21" s="461"/>
+      <c r="C21" s="461"/>
+      <c r="D21" s="462"/>
       <c r="E21" s="279"/>
       <c r="F21" s="279"/>
       <c r="G21" s="279"/>
@@ -19017,10 +17949,10 @@
       </c>
     </row>
     <row r="22" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="455" t="s">
+      <c r="A22" s="469" t="s">
         <v>197</v>
       </c>
-      <c r="B22" s="456"/>
+      <c r="B22" s="470"/>
       <c r="C22" s="160">
         <v>10</v>
       </c>
@@ -19267,12 +18199,12 @@
       </c>
     </row>
     <row r="28" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="470" t="s">
+      <c r="A28" s="460" t="s">
         <v>198</v>
       </c>
-      <c r="B28" s="471"/>
-      <c r="C28" s="471"/>
-      <c r="D28" s="472"/>
+      <c r="B28" s="461"/>
+      <c r="C28" s="461"/>
+      <c r="D28" s="462"/>
       <c r="E28" s="279">
         <f t="shared" ref="E28:T28" si="16">SUM(E22:E27)</f>
         <v>0</v>
@@ -19343,12 +18275,12 @@
       </c>
     </row>
     <row r="29" spans="1:40" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="470" t="s">
+      <c r="A29" s="460" t="s">
         <v>199</v>
       </c>
-      <c r="B29" s="471"/>
-      <c r="C29" s="471"/>
-      <c r="D29" s="472"/>
+      <c r="B29" s="461"/>
+      <c r="C29" s="461"/>
+      <c r="D29" s="462"/>
       <c r="E29" s="279"/>
       <c r="F29" s="279"/>
       <c r="G29" s="279"/>
@@ -19374,10 +18306,10 @@
       </c>
     </row>
     <row r="30" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="455" t="s">
+      <c r="A30" s="469" t="s">
         <v>200</v>
       </c>
-      <c r="B30" s="456"/>
+      <c r="B30" s="470"/>
       <c r="C30" s="160">
         <v>10</v>
       </c>
@@ -19624,12 +18556,12 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="470" t="s">
+      <c r="A36" s="460" t="s">
         <v>201</v>
       </c>
-      <c r="B36" s="471"/>
-      <c r="C36" s="471"/>
-      <c r="D36" s="472"/>
+      <c r="B36" s="461"/>
+      <c r="C36" s="461"/>
+      <c r="D36" s="462"/>
       <c r="E36" s="279">
         <f t="shared" ref="E36:T36" si="17">SUM(E30:E35)</f>
         <v>0</v>
@@ -19700,12 +18632,12 @@
       </c>
     </row>
     <row r="37" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="470" t="s">
+      <c r="A37" s="460" t="s">
         <v>202</v>
       </c>
-      <c r="B37" s="471"/>
-      <c r="C37" s="471"/>
-      <c r="D37" s="472"/>
+      <c r="B37" s="461"/>
+      <c r="C37" s="461"/>
+      <c r="D37" s="462"/>
       <c r="E37" s="279"/>
       <c r="F37" s="279"/>
       <c r="G37" s="279"/>
@@ -19731,10 +18663,10 @@
       </c>
     </row>
     <row r="38" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="455" t="s">
+      <c r="A38" s="469" t="s">
         <v>203</v>
       </c>
-      <c r="B38" s="456"/>
+      <c r="B38" s="470"/>
       <c r="C38" s="160">
         <v>10</v>
       </c>
@@ -19981,12 +18913,12 @@
       </c>
     </row>
     <row r="44" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="470" t="s">
+      <c r="A44" s="460" t="s">
         <v>204</v>
       </c>
-      <c r="B44" s="471"/>
-      <c r="C44" s="471"/>
-      <c r="D44" s="472"/>
+      <c r="B44" s="461"/>
+      <c r="C44" s="461"/>
+      <c r="D44" s="462"/>
       <c r="E44" s="279">
         <f t="shared" ref="E44:T44" si="18">SUM(E38:E43)</f>
         <v>0</v>
@@ -20057,12 +18989,12 @@
       </c>
     </row>
     <row r="45" spans="1:22" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="470" t="s">
+      <c r="A45" s="460" t="s">
         <v>205</v>
       </c>
-      <c r="B45" s="471"/>
-      <c r="C45" s="471"/>
-      <c r="D45" s="472"/>
+      <c r="B45" s="461"/>
+      <c r="C45" s="461"/>
+      <c r="D45" s="462"/>
       <c r="E45" s="279"/>
       <c r="F45" s="279"/>
       <c r="G45" s="279"/>
@@ -20088,11 +19020,11 @@
       </c>
     </row>
     <row r="46" spans="1:22" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="457" t="s">
+      <c r="A46" s="478" t="s">
         <v>206</v>
       </c>
-      <c r="B46" s="458"/>
-      <c r="C46" s="459"/>
+      <c r="B46" s="479"/>
+      <c r="C46" s="480"/>
       <c r="D46" s="170"/>
       <c r="E46" s="287">
         <f t="shared" ref="E46:U46" si="19">SUM(E6:E11,E14:E19,E22:E27,E30:E35,E38:E43)</f>
@@ -20165,12 +19097,12 @@
       <c r="V46" s="240"/>
     </row>
     <row r="47" spans="1:22" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="465" t="s">
+      <c r="A47" s="484" t="s">
         <v>207</v>
       </c>
-      <c r="B47" s="466"/>
-      <c r="C47" s="466"/>
-      <c r="D47" s="467"/>
+      <c r="B47" s="485"/>
+      <c r="C47" s="485"/>
+      <c r="D47" s="486"/>
       <c r="E47" s="288">
         <f>E46</f>
         <v>1500000</v>
@@ -20241,7 +19173,7 @@
     <row r="48" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A48" s="171"/>
       <c r="B48" s="171"/>
-      <c r="C48" s="468" t="s">
+      <c r="C48" s="487" t="s">
         <v>208</v>
       </c>
       <c r="D48" s="172">
@@ -20316,7 +19248,7 @@
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A49" s="171"/>
-      <c r="C49" s="469"/>
+      <c r="C49" s="488"/>
       <c r="D49" s="242">
         <v>37</v>
       </c>
@@ -20387,7 +19319,7 @@
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A50" s="171"/>
-      <c r="C50" s="469"/>
+      <c r="C50" s="488"/>
       <c r="D50" s="242">
         <v>30</v>
       </c>
@@ -20458,7 +19390,7 @@
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A51" s="171"/>
-      <c r="C51" s="469"/>
+      <c r="C51" s="488"/>
       <c r="D51" s="242">
         <v>41</v>
       </c>
@@ -20528,38 +19460,38 @@
       </c>
     </row>
     <row r="52" spans="1:24" ht="22.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="460" t="s">
+      <c r="A52" s="481" t="s">
         <v>209</v>
       </c>
-      <c r="B52" s="461"/>
-      <c r="C52" s="461"/>
-      <c r="D52" s="461"/>
-      <c r="E52" s="461"/>
-      <c r="F52" s="461"/>
-      <c r="G52" s="461"/>
-      <c r="H52" s="461"/>
-      <c r="I52" s="461"/>
-      <c r="J52" s="461"/>
-      <c r="K52" s="461"/>
-      <c r="L52" s="461"/>
-      <c r="M52" s="461"/>
-      <c r="N52" s="461"/>
-      <c r="O52" s="461"/>
-      <c r="P52" s="461"/>
-      <c r="Q52" s="461"/>
-      <c r="R52" s="461"/>
-      <c r="S52" s="461"/>
-      <c r="T52" s="461"/>
-      <c r="U52" s="461"/>
-      <c r="V52" s="461"/>
-      <c r="W52" s="462"/>
+      <c r="B52" s="482"/>
+      <c r="C52" s="482"/>
+      <c r="D52" s="482"/>
+      <c r="E52" s="482"/>
+      <c r="F52" s="482"/>
+      <c r="G52" s="482"/>
+      <c r="H52" s="482"/>
+      <c r="I52" s="482"/>
+      <c r="J52" s="482"/>
+      <c r="K52" s="482"/>
+      <c r="L52" s="482"/>
+      <c r="M52" s="482"/>
+      <c r="N52" s="482"/>
+      <c r="O52" s="482"/>
+      <c r="P52" s="482"/>
+      <c r="Q52" s="482"/>
+      <c r="R52" s="482"/>
+      <c r="S52" s="482"/>
+      <c r="T52" s="482"/>
+      <c r="U52" s="482"/>
+      <c r="V52" s="482"/>
+      <c r="W52" s="483"/>
       <c r="X52" s="240"/>
     </row>
     <row r="53" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="463" t="s">
+      <c r="A53" s="473" t="s">
         <v>210</v>
       </c>
-      <c r="B53" s="464"/>
+      <c r="B53" s="474"/>
       <c r="C53" s="76">
         <v>10</v>
       </c>
@@ -20736,10 +19668,10 @@
       <c r="X57" s="240"/>
     </row>
     <row r="58" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="453" t="s">
+      <c r="A58" s="471" t="s">
         <v>212</v>
       </c>
-      <c r="B58" s="454"/>
+      <c r="B58" s="472"/>
       <c r="C58" s="76">
         <v>10</v>
       </c>
@@ -20921,10 +19853,10 @@
       <c r="X62" s="240"/>
     </row>
     <row r="63" spans="1:24" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="453" t="s">
+      <c r="A63" s="471" t="s">
         <v>213</v>
       </c>
-      <c r="B63" s="454"/>
+      <c r="B63" s="472"/>
       <c r="C63" s="76">
         <v>10</v>
       </c>
@@ -21114,10 +20046,10 @@
       <c r="X67" s="240"/>
     </row>
     <row r="68" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="453" t="s">
+      <c r="A68" s="471" t="s">
         <v>214</v>
       </c>
-      <c r="B68" s="454"/>
+      <c r="B68" s="472"/>
       <c r="C68" s="76">
         <v>10</v>
       </c>
@@ -21295,10 +20227,10 @@
       <c r="X72" s="240"/>
     </row>
     <row r="73" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="453" t="s">
+      <c r="A73" s="471" t="s">
         <v>215</v>
       </c>
-      <c r="B73" s="454"/>
+      <c r="B73" s="472"/>
       <c r="C73" s="76">
         <v>10</v>
       </c>
@@ -21524,10 +20456,10 @@
       <c r="X77" s="240"/>
     </row>
     <row r="78" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="453" t="s">
+      <c r="A78" s="471" t="s">
         <v>217</v>
       </c>
-      <c r="B78" s="454"/>
+      <c r="B78" s="472"/>
       <c r="C78" s="76">
         <v>10</v>
       </c>
@@ -21699,10 +20631,10 @@
       <c r="X82" s="240"/>
     </row>
     <row r="83" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="453" t="s">
+      <c r="A83" s="471" t="s">
         <v>219</v>
       </c>
-      <c r="B83" s="454"/>
+      <c r="B83" s="472"/>
       <c r="C83" s="76">
         <v>10</v>
       </c>
@@ -21874,10 +20806,10 @@
       <c r="X87" s="240"/>
     </row>
     <row r="88" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="453" t="s">
+      <c r="A88" s="471" t="s">
         <v>50</v>
       </c>
-      <c r="B88" s="454"/>
+      <c r="B88" s="472"/>
       <c r="C88" s="76">
         <v>10</v>
       </c>
@@ -22049,10 +20981,10 @@
       <c r="X92" s="240"/>
     </row>
     <row r="93" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="453" t="s">
+      <c r="A93" s="471" t="s">
         <v>222</v>
       </c>
-      <c r="B93" s="454"/>
+      <c r="B93" s="472"/>
       <c r="C93" s="76">
         <v>10</v>
       </c>
@@ -22254,10 +21186,10 @@
       <c r="X97" s="240"/>
     </row>
     <row r="98" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="453" t="s">
+      <c r="A98" s="471" t="s">
         <v>224</v>
       </c>
-      <c r="B98" s="454"/>
+      <c r="B98" s="472"/>
       <c r="C98" s="76">
         <v>10</v>
       </c>
@@ -22449,10 +21381,10 @@
       <c r="X102" s="240"/>
     </row>
     <row r="103" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="453" t="s">
+      <c r="A103" s="471" t="s">
         <v>226</v>
       </c>
-      <c r="B103" s="454"/>
+      <c r="B103" s="472"/>
       <c r="C103" s="76">
         <v>10</v>
       </c>
@@ -22654,10 +21586,10 @@
       <c r="X107" s="240"/>
     </row>
     <row r="108" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A108" s="453" t="s">
+      <c r="A108" s="471" t="s">
         <v>227</v>
       </c>
-      <c r="B108" s="454"/>
+      <c r="B108" s="472"/>
       <c r="C108" s="76">
         <v>10</v>
       </c>
@@ -22859,10 +21791,10 @@
       <c r="X112" s="240"/>
     </row>
     <row r="113" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A113" s="453" t="s">
+      <c r="A113" s="471" t="s">
         <v>228</v>
       </c>
-      <c r="B113" s="454"/>
+      <c r="B113" s="472"/>
       <c r="C113" s="76">
         <v>10</v>
       </c>
@@ -23024,10 +21956,10 @@
       <c r="X117" s="240"/>
     </row>
     <row r="118" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A118" s="453" t="s">
+      <c r="A118" s="471" t="s">
         <v>229</v>
       </c>
-      <c r="B118" s="454"/>
+      <c r="B118" s="472"/>
       <c r="C118" s="76">
         <v>10</v>
       </c>
@@ -23229,10 +22161,10 @@
       <c r="X122" s="240"/>
     </row>
     <row r="123" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A123" s="453" t="s">
+      <c r="A123" s="471" t="s">
         <v>230</v>
       </c>
-      <c r="B123" s="454"/>
+      <c r="B123" s="472"/>
       <c r="C123" s="76">
         <v>10</v>
       </c>
@@ -23434,10 +22366,10 @@
       <c r="X127" s="240"/>
     </row>
     <row r="128" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A128" s="453" t="s">
+      <c r="A128" s="471" t="s">
         <v>231</v>
       </c>
-      <c r="B128" s="454"/>
+      <c r="B128" s="472"/>
       <c r="C128" s="76">
         <v>10</v>
       </c>
@@ -23639,10 +22571,10 @@
       <c r="X132" s="240"/>
     </row>
     <row r="133" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A133" s="453" t="s">
+      <c r="A133" s="471" t="s">
         <v>232</v>
       </c>
-      <c r="B133" s="454"/>
+      <c r="B133" s="472"/>
       <c r="C133" s="76">
         <v>10</v>
       </c>
@@ -23844,10 +22776,10 @@
       <c r="X137" s="240"/>
     </row>
     <row r="138" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A138" s="453" t="s">
+      <c r="A138" s="471" t="s">
         <v>233</v>
       </c>
-      <c r="B138" s="454"/>
+      <c r="B138" s="472"/>
       <c r="C138" s="80">
         <v>10</v>
       </c>
@@ -24057,10 +22989,10 @@
       <c r="X142" s="240"/>
     </row>
     <row r="143" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A143" s="453" t="s">
+      <c r="A143" s="471" t="s">
         <v>237</v>
       </c>
-      <c r="B143" s="454"/>
+      <c r="B143" s="472"/>
       <c r="C143" s="80">
         <v>10</v>
       </c>
@@ -24153,10 +23085,10 @@
       <c r="X144" s="240"/>
     </row>
     <row r="145" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A145" s="463" t="s">
+      <c r="A145" s="473" t="s">
         <v>239</v>
       </c>
-      <c r="B145" s="464"/>
+      <c r="B145" s="474"/>
       <c r="C145" s="76">
         <v>10</v>
       </c>
@@ -24229,10 +23161,10 @@
       <c r="X146" s="240"/>
     </row>
     <row r="147" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A147" s="463" t="s">
+      <c r="A147" s="473" t="s">
         <v>240</v>
       </c>
-      <c r="B147" s="464"/>
+      <c r="B147" s="474"/>
       <c r="C147" s="76">
         <v>10</v>
       </c>
@@ -24330,10 +23262,10 @@
       <c r="X148" s="240"/>
     </row>
     <row r="149" spans="1:24" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A149" s="463" t="s">
+      <c r="A149" s="473" t="s">
         <v>241</v>
       </c>
-      <c r="B149" s="464"/>
+      <c r="B149" s="474"/>
       <c r="C149" s="76">
         <v>10</v>
       </c>
@@ -24455,12 +23387,12 @@
       <c r="X151" s="240"/>
     </row>
     <row r="152" spans="1:24" ht="13.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A152" s="473" t="s">
+      <c r="A152" s="475" t="s">
         <v>242</v>
       </c>
-      <c r="B152" s="474"/>
-      <c r="C152" s="474"/>
-      <c r="D152" s="475"/>
+      <c r="B152" s="476"/>
+      <c r="C152" s="476"/>
+      <c r="D152" s="477"/>
       <c r="E152" s="311">
         <f t="shared" ref="E152:T152" si="25">SUM(E53:E151)</f>
         <v>5075324</v>
@@ -25072,37 +24004,6 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="E4:U4"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A4:B5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="A149:B149"/>
-    <mergeCell ref="A152:D152"/>
-    <mergeCell ref="A138:B138"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="A133:B133"/>
     <mergeCell ref="A78:B78"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A30:B30"/>
@@ -25119,6 +24020,37 @@
     <mergeCell ref="A44:D44"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A138:B138"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="A149:B149"/>
+    <mergeCell ref="A152:D152"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="E4:U4"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A4:B5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" scale="79" fitToHeight="0" orientation="landscape"/>
@@ -25197,69 +24129,69 @@
       <c r="BZ1" s="186"/>
     </row>
     <row r="2" spans="1:78" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="476" t="s">
+      <c r="A2" s="453" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="496"/>
-      <c r="C2" s="497"/>
-      <c r="D2" s="499" t="s">
+      <c r="B2" s="489"/>
+      <c r="C2" s="490"/>
+      <c r="D2" s="492" t="s">
         <v>351</v>
       </c>
-      <c r="E2" s="500"/>
-      <c r="F2" s="500"/>
-      <c r="G2" s="500"/>
-      <c r="H2" s="500"/>
-      <c r="I2" s="500"/>
-      <c r="J2" s="500"/>
-      <c r="K2" s="500"/>
-      <c r="L2" s="500"/>
-      <c r="M2" s="500"/>
-      <c r="N2" s="500"/>
-      <c r="O2" s="500"/>
-      <c r="P2" s="500"/>
-      <c r="Q2" s="500"/>
-      <c r="R2" s="500"/>
-      <c r="S2" s="500"/>
-      <c r="T2" s="500"/>
+      <c r="E2" s="493"/>
+      <c r="F2" s="493"/>
+      <c r="G2" s="493"/>
+      <c r="H2" s="493"/>
+      <c r="I2" s="493"/>
+      <c r="J2" s="493"/>
+      <c r="K2" s="493"/>
+      <c r="L2" s="493"/>
+      <c r="M2" s="493"/>
+      <c r="N2" s="493"/>
+      <c r="O2" s="493"/>
+      <c r="P2" s="493"/>
+      <c r="Q2" s="493"/>
+      <c r="R2" s="493"/>
+      <c r="S2" s="493"/>
+      <c r="T2" s="493"/>
       <c r="AA2" s="131"/>
       <c r="BY2" s="186"/>
       <c r="BZ2" s="186"/>
     </row>
     <row r="3" spans="1:78" s="20" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="478" t="s">
+      <c r="A3" s="455" t="s">
         <v>172</v>
       </c>
-      <c r="B3" s="496"/>
-      <c r="C3" s="497"/>
+      <c r="B3" s="489"/>
+      <c r="C3" s="490"/>
       <c r="D3" s="52"/>
       <c r="E3" s="53"/>
-      <c r="F3" s="501" t="s">
+      <c r="F3" s="494" t="s">
         <v>352</v>
       </c>
-      <c r="G3" s="502"/>
-      <c r="H3" s="503" t="s">
+      <c r="G3" s="495"/>
+      <c r="H3" s="496" t="s">
         <v>353</v>
       </c>
-      <c r="I3" s="503"/>
-      <c r="J3" s="504"/>
-      <c r="K3" s="505" t="s">
+      <c r="I3" s="496"/>
+      <c r="J3" s="497"/>
+      <c r="K3" s="498" t="s">
         <v>354</v>
       </c>
-      <c r="L3" s="506"/>
-      <c r="M3" s="507"/>
-      <c r="N3" s="504" t="s">
+      <c r="L3" s="499"/>
+      <c r="M3" s="500"/>
+      <c r="N3" s="497" t="s">
         <v>355</v>
       </c>
-      <c r="O3" s="508"/>
-      <c r="P3" s="509"/>
-      <c r="Q3" s="510" t="s">
+      <c r="O3" s="501"/>
+      <c r="P3" s="502"/>
+      <c r="Q3" s="503" t="s">
         <v>356</v>
       </c>
-      <c r="R3" s="511"/>
-      <c r="S3" s="512" t="s">
+      <c r="R3" s="504"/>
+      <c r="S3" s="505" t="s">
         <v>357</v>
       </c>
-      <c r="T3" s="513"/>
+      <c r="T3" s="506"/>
       <c r="AA3" s="132"/>
     </row>
     <row r="4" spans="1:78" s="20" customFormat="1" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -25424,7 +24356,7 @@
       <c r="AC6" s="133"/>
     </row>
     <row r="7" spans="1:78" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="490" t="str">
+      <c r="C7" s="511" t="str">
         <f>"Projected Annual Cost
 "&amp;D5&amp;" Dollar Year" &amp;"
 ($Million)"</f>
@@ -25432,81 +24364,81 @@
 2020 Dollar Year
 ($Million)</v>
       </c>
-      <c r="D7" s="491"/>
-      <c r="E7" s="492"/>
-      <c r="F7" s="491" t="s">
+      <c r="D7" s="514"/>
+      <c r="E7" s="512"/>
+      <c r="F7" s="514" t="s">
         <v>380</v>
       </c>
-      <c r="G7" s="491"/>
-      <c r="H7" s="492"/>
-      <c r="I7" s="493" t="str">
+      <c r="G7" s="514"/>
+      <c r="H7" s="512"/>
+      <c r="I7" s="515" t="str">
         <f>"Projected Annual Cost with Financing
 ($Million; NPV=$"&amp;ROUND(Q52,3)&amp;")"</f>
         <v>Projected Annual Cost with Financing
 ($Million; NPV=$2606.746)</v>
       </c>
-      <c r="J7" s="494"/>
-      <c r="K7" s="494"/>
-      <c r="L7" s="494"/>
-      <c r="M7" s="494"/>
-      <c r="N7" s="494"/>
-      <c r="O7" s="494"/>
-      <c r="P7" s="494"/>
-      <c r="Q7" s="494"/>
-      <c r="R7" s="495"/>
-      <c r="S7" s="490" t="str">
+      <c r="J7" s="516"/>
+      <c r="K7" s="516"/>
+      <c r="L7" s="516"/>
+      <c r="M7" s="516"/>
+      <c r="N7" s="516"/>
+      <c r="O7" s="516"/>
+      <c r="P7" s="516"/>
+      <c r="Q7" s="516"/>
+      <c r="R7" s="517"/>
+      <c r="S7" s="511" t="str">
         <f>"Avoided MWD Purchase 
  ($Million; NPV=$"&amp;ROUND(Y52,3)&amp;")"</f>
         <v>Avoided MWD Purchase 
  ($Million; NPV=$125.07)</v>
       </c>
-      <c r="T7" s="491"/>
-      <c r="U7" s="491"/>
-      <c r="V7" s="491"/>
-      <c r="W7" s="491"/>
-      <c r="X7" s="492"/>
-      <c r="Y7" s="490" t="s">
+      <c r="T7" s="514"/>
+      <c r="U7" s="514"/>
+      <c r="V7" s="514"/>
+      <c r="W7" s="514"/>
+      <c r="X7" s="512"/>
+      <c r="Y7" s="511" t="s">
         <v>381</v>
       </c>
-      <c r="Z7" s="492"/>
+      <c r="Z7" s="512"/>
       <c r="AA7" s="134"/>
-      <c r="AH7" s="514" t="s">
+      <c r="AH7" s="507" t="s">
         <v>382</v>
       </c>
-      <c r="AI7" s="515"/>
+      <c r="AI7" s="508"/>
       <c r="AJ7" s="13"/>
-      <c r="AK7" s="516" t="s">
+      <c r="AK7" s="509" t="s">
         <v>383</v>
       </c>
       <c r="AL7" s="452"/>
       <c r="AM7" s="452"/>
-      <c r="AN7" s="515"/>
-      <c r="AP7" s="517" t="s">
+      <c r="AN7" s="508"/>
+      <c r="AP7" s="510" t="s">
         <v>384</v>
       </c>
-      <c r="AQ7" s="482"/>
-      <c r="AS7" s="498" t="s">
+      <c r="AQ7" s="459"/>
+      <c r="AS7" s="491" t="s">
         <v>385</v>
       </c>
-      <c r="AT7" s="481"/>
-      <c r="AU7" s="481"/>
-      <c r="AV7" s="481"/>
-      <c r="AW7" s="481"/>
-      <c r="AX7" s="481"/>
-      <c r="AY7" s="481"/>
-      <c r="AZ7" s="481"/>
-      <c r="BA7" s="481"/>
-      <c r="BB7" s="482"/>
-      <c r="BD7" s="517" t="s">
+      <c r="AT7" s="458"/>
+      <c r="AU7" s="458"/>
+      <c r="AV7" s="458"/>
+      <c r="AW7" s="458"/>
+      <c r="AX7" s="458"/>
+      <c r="AY7" s="458"/>
+      <c r="AZ7" s="458"/>
+      <c r="BA7" s="458"/>
+      <c r="BB7" s="459"/>
+      <c r="BD7" s="510" t="s">
         <v>386</v>
       </c>
-      <c r="BE7" s="482"/>
+      <c r="BE7" s="459"/>
       <c r="BF7" s="186"/>
-      <c r="BG7" s="498" t="s">
+      <c r="BG7" s="491" t="s">
         <v>387</v>
       </c>
-      <c r="BH7" s="481"/>
-      <c r="BI7" s="481"/>
+      <c r="BH7" s="458"/>
+      <c r="BI7" s="458"/>
       <c r="BY7" s="186"/>
       <c r="BZ7" s="186"/>
     </row>
@@ -35451,17 +34383,17 @@
       <c r="BZ52" s="186"/>
     </row>
     <row r="53" spans="1:78" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C53" s="489"/>
-      <c r="D53" s="489"/>
-      <c r="E53" s="489"/>
-      <c r="F53" s="489"/>
-      <c r="G53" s="489"/>
-      <c r="H53" s="489"/>
-      <c r="I53" s="489"/>
-      <c r="J53" s="489"/>
-      <c r="K53" s="489"/>
-      <c r="L53" s="489"/>
-      <c r="M53" s="489"/>
+      <c r="C53" s="513"/>
+      <c r="D53" s="513"/>
+      <c r="E53" s="513"/>
+      <c r="F53" s="513"/>
+      <c r="G53" s="513"/>
+      <c r="H53" s="513"/>
+      <c r="I53" s="513"/>
+      <c r="J53" s="513"/>
+      <c r="K53" s="513"/>
+      <c r="L53" s="513"/>
+      <c r="M53" s="513"/>
       <c r="AC53" s="136" t="s">
         <v>436</v>
       </c>
@@ -35600,6 +34532,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C53:M53"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:R7"/>
+    <mergeCell ref="S7:X7"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="BG7:BI7"/>
@@ -35616,11 +34553,6 @@
     <mergeCell ref="AS7:BB7"/>
     <mergeCell ref="BD7:BE7"/>
     <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="C53:M53"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:R7"/>
-    <mergeCell ref="S7:X7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="5">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="N5 S5 X6" xr:uid="{00000000-0002-0000-0800-000000000000}">
@@ -50190,7 +49122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3141C089-AF0B-F64C-88A5-21CA43370521}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>